<commit_message>
Standardize file paths for scripts 2 through 18
</commit_message>
<xml_diff>
--- a/docs/script_pipeline.xlsx
+++ b/docs/script_pipeline.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qread\Documents\GitHub\foodwaste\virtualland\scenario_analysis_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qread\Documents\GitHub\foodwaste\biodiversity-farm2fork-analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="166">
   <si>
     <t>Section</t>
   </si>
   <si>
-    <t>Order to run</t>
-  </si>
-  <si>
     <t>Script name</t>
   </si>
   <si>
@@ -48,18 +45,12 @@
     <t>main domestic analysis</t>
   </si>
   <si>
-    <t>county_downscale_nass_cbp.R</t>
-  </si>
-  <si>
     <t>nass_workers_receipts_3landtypes_bea.csv</t>
   </si>
   <si>
     <t>by state and BEA, commodity receipts, number of employees, and land area of annual crop, permanent crop, and pasture</t>
   </si>
   <si>
-    <t>downscale_state_production_county.R</t>
-  </si>
-  <si>
     <t>Use the county-level weightings to downscale state-level production of goods to the county level, based on numbers of establishments in each county</t>
   </si>
   <si>
@@ -69,9 +60,6 @@
     <t>Downscaled production vector by BEA code by county</t>
   </si>
   <si>
-    <t>land_exchange_by_state.R</t>
-  </si>
-  <si>
     <t>Divide the land areas by the total commodity receipts for each BEA code for each state to get a "land exchange" or I-O model coefficient matrix for each state.</t>
   </si>
   <si>
@@ -90,9 +78,6 @@
     <t>processed USA dietary guidelines 2015</t>
   </si>
   <si>
-    <t>healthy_diet_simulation.R</t>
-  </si>
-  <si>
     <t>Further process the diet data, converting everything to calories so they are in common units, then joining it with LAFA based on a crosswalk table</t>
   </si>
   <si>
@@ -108,9 +93,6 @@
     <t>Lancet and USA dietary guidelines data all converted to the same units; LAFA joined with the diet data</t>
   </si>
   <si>
-    <t>waste_reduction_simulation.R</t>
-  </si>
-  <si>
     <t>Use the preconsumer and consumer waste estimates from LAFA to add waste reduction factors to the diet factors in the joined LAFA-diet data</t>
   </si>
   <si>
@@ -126,9 +108,6 @@
     <t>Factors, relative to baseline, representing the change in food consumption for each LAFA category under alternative diet scenarios and waste reduction scenarios. Now a separate one is done for domestic and foreign.</t>
   </si>
   <si>
-    <t>harmonize_scenarios_bea.R</t>
-  </si>
-  <si>
     <t>Map the LAFA categories to BEA categories, then calculate the consumption factors for diet scenarios, waste reduction scenarios, and factorial combination of the two, for each BEA category. This requires supplementing the LAFA data and diet data with assumptions for change in beverage consumption which isn't included in either LAFA or explicitly in the diet data.</t>
   </si>
   <si>
@@ -144,9 +123,6 @@
     <t>Food consumption factors relative to baseline for all food-related BEA codes in all diet scenarios, waste scenarios, and diet x waste scenarios</t>
   </si>
   <si>
-    <t>county_level_consumption.R</t>
-  </si>
-  <si>
     <t>First use the county-level personal income data to downscale the BEA baseline personal consumption expenditures vector to each county. Then, use the consumption factors to create an alternative vector for each county in each scenario. Next, apply the I-O approach by multiplying the Leontief inverse by the vector for each county to get the total demand from each county in each scenario, including intermediate.</t>
   </si>
   <si>
@@ -159,9 +135,6 @@
     <t>downscaled personal consumption expenditure vector for each county in each scenario; total demand vector (intermediate + final) for each county in each scenario. Includes all goods, not just agricultural.</t>
   </si>
   <si>
-    <t>county_allocate_flows_simple.R</t>
-  </si>
-  <si>
     <t>Use the assumption that production of each county is proportionally allocated to all counties, ignoring the distance between them. For all counties, BEA categories, and scenarios, allocate all county production to a consuming county.</t>
   </si>
   <si>
@@ -171,9 +144,6 @@
     <t>inter-county flows of agricultural goods for each BEA category in each scenario</t>
   </si>
   <si>
-    <t>land_footprint_estimate.R; newer version land_footprint_estimate_DT.R</t>
-  </si>
-  <si>
     <t>Apply the second part of the EEIO model by multiplying the county total demand for each county in each scenario) allocated across all producing counties, times the land exchanges for the states where the producing counties are located, to result in land flows between each county in each scenario (including 3 land types).</t>
   </si>
   <si>
@@ -189,9 +159,6 @@
     <t>inter-county flows of land, in 3 categories, in each scenario</t>
   </si>
   <si>
-    <t>county_to_tnc_landflows.R; new version county_to_tnc_landflows_DT.R (see also the version county_landflows_weight_tnc_DT.R in DT_version/deprecated/ folder)</t>
-  </si>
-  <si>
     <t>Convert flows from inter-county flows to inter-TNC ecoregion flows (first incoming only, or TNC to county, and next incoming+outgoing, or TNC to TNC). The first part is done by proportionally dividing up the flows exiting each county to flows exiting each TNC ecoregion that makes up that county, based on the proportions of NLCD pixels in each ecoregion in each county. The second part is done by proportionally dividing up the flows entering each county to flows entering each TNC ecoregion that makes up that county, based on the proportion of population in each ecoregion in each county. (Those proportional counts were done in previous scripts described elsewhere.)</t>
   </si>
   <si>
@@ -207,9 +174,6 @@
     <t>flows of land from each TNC ecoregion to each county in each scenario; inter-ecoregion flows of land in each scenario (separate files for each scenario, and combined into one)</t>
   </si>
   <si>
-    <t>landflows_to_biodiv.R; newer version landflows_to_biodiv_by_county_DT.R</t>
-  </si>
-  <si>
     <t>Multiply inter-TNC-ecoregion flows by biodiversity threat characterization factors to get the estimated species lost as a result of each flow. This is done by joining the TNC-TNC flow data for each scenario with the Chaudhary characterization factors for the TNC region where the flow originates, using the "medium intensity" assumption, then multiplying the flow in square meters by the CF in species lost per square meter of land occupied.</t>
   </si>
   <si>
@@ -228,9 +192,6 @@
     <t>foreign analysis</t>
   </si>
   <si>
-    <t>fao_foreign_land_imports_DT.R</t>
-  </si>
-  <si>
     <t>Find how much cropland and pastureland is imported from foreign countries to United States under baseline and alternative scenario</t>
   </si>
   <si>
@@ -246,9 +207,6 @@
     <t>production of crops and animal products in foreign countries and quantities of each sent to USA; exports to USA converted to virtual land transfers</t>
   </si>
   <si>
-    <t>fao_transfers_by_ecoregion_DT.R</t>
-  </si>
-  <si>
     <t>Proportionally allocate the virtual land flows from exporting countries to ecoregions within those countries</t>
   </si>
   <si>
@@ -264,9 +222,6 @@
     <t>foreign virtual land transfers originating from each combination of country x TNC ecoregion; the same summed by ecoregion</t>
   </si>
   <si>
-    <t>foreign_vlt_to_counties_DT.R</t>
-  </si>
-  <si>
     <t>Allocate imported virtual land flows to importing counties, assuming for simplification that they are distributed proportionally based on county income</t>
   </si>
   <si>
@@ -282,9 +237,6 @@
     <t>foreign virtual land transfers by exporting ecoregion by importing county; the same summed for each importing county</t>
   </si>
   <si>
-    <t>foreign_landflows_to_biodiv_DT.R</t>
-  </si>
-  <si>
     <t>Use Chaudhary's characterization factors to convert the virtual land flows to biodiversity flows by exporting ecoregion and importing county</t>
   </si>
   <si>
@@ -303,33 +255,6 @@
     <t>visualizations</t>
   </si>
   <si>
-    <t>figs/figs_v2_summarydata.R</t>
-  </si>
-  <si>
-    <t>Calculate high level sums of flows for plotting; smaller ones that can be run locally</t>
-  </si>
-  <si>
-    <t>figs/figs_v2_summarydata_parallel.R</t>
-  </si>
-  <si>
-    <t>Calculate high level sums of flows for plotting; larger ones that require parallel procesisng, including flows of land and goods for all counties across all scenarios</t>
-  </si>
-  <si>
-    <t>figs/figs_v2_loaddata.R (sources figs_v2_lookups.R)</t>
-  </si>
-  <si>
-    <t>Loads all necessary data, map objects, lookup tables, and plotting themes for making figures</t>
-  </si>
-  <si>
-    <t>All other scripts prefixed figs/figs_v2_X.R; includes consumption, countylandmaps, ecoregionmaps, foreign, panelmaps, statectyextmaps</t>
-  </si>
-  <si>
-    <t>disaggregate_oilseed_grain.R</t>
-  </si>
-  <si>
-    <t>get_useeio_components.R</t>
-  </si>
-  <si>
     <t>none (all data present in useeior package)</t>
   </si>
   <si>
@@ -381,12 +306,6 @@
     <t>downscaled total demand vector for each county in each scenario; downscaled production vector for each county (relative differences in production do not change by scenario)</t>
   </si>
   <si>
-    <t>extract_faostat.R</t>
-  </si>
-  <si>
-    <t>extract_fbs.R</t>
-  </si>
-  <si>
     <t>process raw FAOSTAT data into usable format, averaging the past 5 years of data for all data points</t>
   </si>
   <si>
@@ -426,9 +345,6 @@
     <t>spatial processing</t>
   </si>
   <si>
-    <t>spatial/spatial_processing.Rmd</t>
-  </si>
-  <si>
     <t>Code notebook combining several scripts. All vector and raster files are transformed to appropriate projections. Intersect TNC ecoregions with both countries and counties. Summarize pixel counts of NLCD and population by TNC-county intersect, and counts of global crop and pasture rasters by TNC-country intersect.</t>
   </si>
   <si>
@@ -441,9 +357,6 @@
     <t>raw_data/commodity_flows/Lin_supp_info/County Personal Income.xlsx; useeio2012v2.0_pce_drc.RData; bea_consumption_factors_diet_waste_scenarios.csv</t>
   </si>
   <si>
-    <t>read_clean_lafa_data.R</t>
-  </si>
-  <si>
     <t>data/raw_data/USDA/LAFA/*.xls</t>
   </si>
   <si>
@@ -453,9 +366,6 @@
     <t>lafa_cleaned.csv</t>
   </si>
   <si>
-    <t>read_chaudh2018_si.R</t>
-  </si>
-  <si>
     <t>Convert supplementary information from Chaudhary and Brooks 2018 (biodiversity characterization factors) to clean form</t>
   </si>
   <si>
@@ -477,9 +387,6 @@
     <t>data pre-processing</t>
   </si>
   <si>
-    <t>read_qfahpd_data.R</t>
-  </si>
-  <si>
     <t>Convert raw LAFA data to a single data frame and write to CSV</t>
   </si>
   <si>
@@ -504,13 +411,112 @@
     <t>Listed in data sources under spatial data, and crosswalk to harmonize county map with county data</t>
   </si>
   <si>
-    <t>read_usdadiet2025.R</t>
-  </si>
-  <si>
     <t>dietaryguidelines2020-2025cleaned.xlsx</t>
   </si>
   <si>
     <t>us_dietary_guidelines2020-2025_wide.csv; us_dietary_guidelines2020-2025_long.csv</t>
+  </si>
+  <si>
+    <t>01_spatial_processing.Rmd</t>
+  </si>
+  <si>
+    <t>02_read_qfahpd_data.R</t>
+  </si>
+  <si>
+    <t>03_read_clean_lafa_data.R</t>
+  </si>
+  <si>
+    <t>04_read_chaudh2018_si.R</t>
+  </si>
+  <si>
+    <t>06_disaggregate_oilseed_grain.R</t>
+  </si>
+  <si>
+    <t>05_get_useeio_components.R</t>
+  </si>
+  <si>
+    <t>07_county_downscale_nass_cbp.R</t>
+  </si>
+  <si>
+    <t>08_downscale_state_production_county.R</t>
+  </si>
+  <si>
+    <t>09_land_exchange_by_state.R</t>
+  </si>
+  <si>
+    <t>10_read_usdadiet2025.R</t>
+  </si>
+  <si>
+    <t>11_healthy_diet_simulation.R</t>
+  </si>
+  <si>
+    <t>12_waste_reduction_simulation.R</t>
+  </si>
+  <si>
+    <t>13_harmonize_scenarios_bea.R</t>
+  </si>
+  <si>
+    <t>14_county_level_consumption.R</t>
+  </si>
+  <si>
+    <t>15_county_allocate_flows_simple.R</t>
+  </si>
+  <si>
+    <t>16_land_footprint_estimate.R</t>
+  </si>
+  <si>
+    <t>17_county_to_tnc_landflows.R</t>
+  </si>
+  <si>
+    <t>18_landflows_to_biodiv_by_county.R</t>
+  </si>
+  <si>
+    <t>19_extract_faostat.R</t>
+  </si>
+  <si>
+    <t>20_extract_fbs.R</t>
+  </si>
+  <si>
+    <t>21_fao_foreign_land_imports.R</t>
+  </si>
+  <si>
+    <t>22_fao_transfers_by_ecoregion.R</t>
+  </si>
+  <si>
+    <t>23_foreign_vlt_to_counties.R</t>
+  </si>
+  <si>
+    <t>24_foreign_landflows_to_biodiv.R</t>
+  </si>
+  <si>
+    <t>25_create_summary_data.R</t>
+  </si>
+  <si>
+    <t>Calculate high level sums of flows for plotting; smaller ones are run sequentially and larger ones require parallel processing (flows of land and goods for all counties across all scenarios)</t>
+  </si>
+  <si>
+    <t>26_compile_Shiny_data.R</t>
+  </si>
+  <si>
+    <t>Process data for Shiny app</t>
+  </si>
+  <si>
+    <t>Figure scripts</t>
+  </si>
+  <si>
+    <t>Scripts called fig(x).r create that number figure in the manuscript, and scripts prefixed supplemental_figs_ create figures that appear in supplements. These scripts source other scripts prefixed load_data*.R and us_map_fxns.R which load data and functions.</t>
+  </si>
+  <si>
+    <t>Table scripts</t>
+  </si>
+  <si>
+    <t>The three scripts in the tables directory produce the tables that appear in the supplemental tables document.</t>
+  </si>
+  <si>
+    <t>Supplemental Rmd notebooks</t>
+  </si>
+  <si>
+    <t>the two Rmd notebooks in the supplements directory produce the supplemental figures and supplemental tables PDF documents.</t>
   </si>
 </sst>
 </file>
@@ -1321,728 +1327,654 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="31" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="2" t="s">
+    </row>
+    <row r="28" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="2" t="s">
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="255" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="2" t="s">
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26">
-        <v>25</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27">
-        <v>26</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28">
-        <v>27</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29">
-        <v>28</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>100</v>
+      <c r="B30" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>